<commit_message>
Anil changes on Payment
Anil changes on Payment
</commit_message>
<xml_diff>
--- a/Src/ACQ.Web.App/ExcelFile/StageDetails.xlsx
+++ b/Src/ACQ.Web.App/ExcelFile/StageDetails.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anil Kumar\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>ContractmasterId</t>
   </si>
@@ -83,20 +78,23 @@
     <t>BCD0013</t>
   </si>
   <si>
-    <t>BCD0014</t>
-  </si>
-  <si>
     <t>ExpendMadeTill31March</t>
   </si>
   <si>
     <t>Part</t>
+  </si>
+  <si>
+    <t>BCD0015</t>
+  </si>
+  <si>
+    <t>BCD0019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,7 +195,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -232,7 +230,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -409,40 +407,40 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" customWidth="1"/>
-    <col min="6" max="6" width="20.88671875" customWidth="1"/>
-    <col min="7" max="7" width="23.109375" customWidth="1"/>
+    <col min="1" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
     <col min="8" max="8" width="16" style="4" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="20.33203125" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" customWidth="1"/>
     <col min="13" max="13" width="23" customWidth="1"/>
-    <col min="14" max="14" width="18.88671875" customWidth="1"/>
-    <col min="15" max="15" width="28.33203125" customWidth="1"/>
-    <col min="16" max="16" width="20.109375" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" customWidth="1"/>
+    <col min="15" max="15" width="28.28515625" customWidth="1"/>
+    <col min="16" max="16" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,10 +487,10 @@
         <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>1</v>
       </c>
@@ -536,13 +534,13 @@
         <v>1000</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P2">
         <v>100.2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>1</v>
       </c>
@@ -550,7 +548,7 @@
         <v>18</v>
       </c>
       <c r="C3">
-        <v>230244</v>
+        <v>230245</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -586,13 +584,13 @@
         <v>1000</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P3">
         <v>100.2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>1</v>
       </c>
@@ -600,7 +598,7 @@
         <v>18</v>
       </c>
       <c r="C4">
-        <v>230244</v>
+        <v>230246</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -636,21 +634,21 @@
         <v>1000</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P4">
         <v>100.2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C5">
-        <v>230244</v>
+        <v>2302412</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -686,21 +684,21 @@
         <v>1000</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P5">
         <v>100.2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C6">
-        <v>230244</v>
+        <v>2302421</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -736,21 +734,21 @@
         <v>1000</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P6">
         <v>100.2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C7">
-        <v>230244</v>
+        <v>2302422</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -786,7 +784,7 @@
         <v>1000</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P7">
         <v>100.2</v>

</xml_diff>

<commit_message>
Commit abid 5th may
</commit_message>
<xml_diff>
--- a/Src/ACQ.Web.App/ExcelFile/StageDetails.xlsx
+++ b/Src/ACQ.Web.App/ExcelFile/StageDetails.xlsx
@@ -24,7 +24,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
+  <si>
+    <t>ContractmasterId</t>
+  </si>
   <si>
     <t>StageNumber</t>
   </si>
@@ -50,19 +53,43 @@
     <t>Conditions</t>
   </si>
   <si>
+    <t>RevisedDateOfpayment</t>
+  </si>
+  <si>
+    <t>ReasonsForSlippage</t>
+  </si>
+  <si>
+    <t>ActualDateOfPayment</t>
+  </si>
+  <si>
+    <t>TotalPaymentMade</t>
+  </si>
+  <si>
+    <t>FullorPartPaymentMade</t>
+  </si>
+  <si>
     <t>Hi this is description</t>
   </si>
   <si>
     <t>Hi this is conditions</t>
   </si>
   <si>
+    <t xml:space="preserve">Hi, My reason isd that </t>
+  </si>
+  <si>
     <t>ContractId</t>
   </si>
   <si>
     <t>BCD0013</t>
   </si>
   <si>
-    <t>BCD0015</t>
+    <t>BCD0014</t>
+  </si>
+  <si>
+    <t>ExpendMadeTill31March</t>
+  </si>
+  <si>
+    <t>Part</t>
   </si>
 </sst>
 </file>
@@ -390,31 +417,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" customWidth="1"/>
-    <col min="7" max="7" width="16" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+    <col min="1" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" customWidth="1"/>
+    <col min="7" max="7" width="23.109375" customWidth="1"/>
+    <col min="8" max="8" width="16" style="4" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
+    <col min="14" max="14" width="18.88671875" customWidth="1"/>
+    <col min="15" max="15" width="28.33203125" customWidth="1"/>
+    <col min="16" max="16" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -428,188 +461,335 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
         <v>230244</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2">
-        <v>44295</v>
+      <c r="D2" t="s">
+        <v>14</v>
       </c>
       <c r="E2" s="2">
         <v>44295</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
+        <v>44295</v>
+      </c>
+      <c r="G2">
         <v>10</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="4">
         <v>505</v>
       </c>
-      <c r="H2" s="2">
-        <v>44295</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
+      <c r="I2" s="2">
+        <v>44295</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2">
+        <v>44295</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="2">
+        <v>44295</v>
+      </c>
+      <c r="N2">
+        <v>1000</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2">
+        <v>100.2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
         <v>230244</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2">
-        <v>44295</v>
+      <c r="D3" t="s">
+        <v>14</v>
       </c>
       <c r="E3" s="2">
         <v>44295</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
+        <v>44295</v>
+      </c>
+      <c r="G3">
         <v>10</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>505</v>
       </c>
-      <c r="H3" s="2">
-        <v>44295</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
+      <c r="I3" s="2">
+        <v>44295</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="2">
+        <v>44295</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="2">
+        <v>44295</v>
+      </c>
+      <c r="N3">
+        <v>1000</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3">
+        <v>100.2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
         <v>230244</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2">
-        <v>44295</v>
+      <c r="D4" t="s">
+        <v>14</v>
       </c>
       <c r="E4" s="2">
         <v>44295</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
+        <v>44295</v>
+      </c>
+      <c r="G4">
         <v>10</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>505</v>
       </c>
-      <c r="H4" s="2">
-        <v>44295</v>
-      </c>
-      <c r="I4" t="s">
-        <v>9</v>
+      <c r="I4" s="2">
+        <v>44295</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="2">
+        <v>44295</v>
+      </c>
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="2">
+        <v>44295</v>
+      </c>
+      <c r="N4">
+        <v>1000</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4">
+        <v>100.2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
         <v>230244</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2">
-        <v>44295</v>
+      <c r="D5" t="s">
+        <v>14</v>
       </c>
       <c r="E5" s="2">
         <v>44295</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
+        <v>44295</v>
+      </c>
+      <c r="G5">
         <v>10</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="4">
         <v>505</v>
       </c>
-      <c r="H5" s="2">
-        <v>44295</v>
-      </c>
-      <c r="I5" t="s">
-        <v>9</v>
+      <c r="I5" s="2">
+        <v>44295</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="2">
+        <v>44295</v>
+      </c>
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="2">
+        <v>44295</v>
+      </c>
+      <c r="N5">
+        <v>1000</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5">
+        <v>100.2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
         <v>230244</v>
       </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2">
-        <v>44295</v>
+      <c r="D6" t="s">
+        <v>14</v>
       </c>
       <c r="E6" s="2">
         <v>44295</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
+        <v>44295</v>
+      </c>
+      <c r="G6">
         <v>10</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="4">
         <v>505</v>
       </c>
-      <c r="H6" s="2">
-        <v>44295</v>
-      </c>
-      <c r="I6" t="s">
-        <v>9</v>
+      <c r="I6" s="2">
+        <v>44295</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="2">
+        <v>44295</v>
+      </c>
+      <c r="L6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="2">
+        <v>44295</v>
+      </c>
+      <c r="N6">
+        <v>1000</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6">
+        <v>100.2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
         <v>230244</v>
       </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2">
-        <v>44295</v>
+      <c r="D7" t="s">
+        <v>14</v>
       </c>
       <c r="E7" s="2">
         <v>44295</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
+        <v>44295</v>
+      </c>
+      <c r="G7">
         <v>10</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7" s="4">
         <v>505</v>
       </c>
-      <c r="H7" s="2">
-        <v>44295</v>
-      </c>
-      <c r="I7" t="s">
-        <v>9</v>
+      <c r="I7" s="2">
+        <v>44295</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="2">
+        <v>44295</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="2">
+        <v>44295</v>
+      </c>
+      <c r="N7">
+        <v>1000</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7">
+        <v>100.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>